<commit_message>
working on integrating new wind incentives -- #495
</commit_message>
<xml_diff>
--- a/data_share/wind_incentives_update_2016_01_22/Data/Output/curated_incentives/column_lookup.xlsx
+++ b/data_share/wind_incentives_update_2016_01_22/Data/Output/curated_incentives/column_lookup.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26423"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="19200" windowHeight="21160" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="27">
   <si>
     <t>incentive_type</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>max_aep_kwh</t>
-  </si>
-  <si>
-    <t>duration_yrs</t>
   </si>
 </sst>
 </file>
@@ -491,10 +488,16 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="18.83203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -732,7 +735,7 @@
     </row>
     <row r="13" spans="1:6">
       <c r="B13" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>6</v>

</xml_diff>